<commit_message>
Implemented Login & Restrict Access to Certain Pages
</commit_message>
<xml_diff>
--- a/Group 68 Burndown Charts.xlsx
+++ b/Group 68 Burndown Charts.xlsx
@@ -587,6 +587,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4188,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4400,6 +4403,9 @@
       <c r="B35" s="3">
         <f t="shared" si="0"/>
         <v>21.600000000000016</v>
+      </c>
+      <c r="C35" s="1">
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Data Flow Diagrams, Updated Burndown Charts
</commit_message>
<xml_diff>
--- a/Group 68 Burndown Charts.xlsx
+++ b/Group 68 Burndown Charts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -551,10 +551,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn down chart'!$C$24:$C$36</c:f>
+              <c:f>'Burn down chart'!$C$24:$C$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>48</c:v>
                 </c:pt>
@@ -593,6 +593,27 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4194,8 +4215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4443,6 +4464,9 @@
         <f t="shared" si="0"/>
         <v>14.400000000000018</v>
       </c>
+      <c r="C38" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
@@ -4452,6 +4476,9 @@
         <f t="shared" si="0"/>
         <v>12.000000000000018</v>
       </c>
+      <c r="C39" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
@@ -4461,6 +4488,9 @@
         <f t="shared" si="0"/>
         <v>9.6000000000000174</v>
       </c>
+      <c r="C40" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
@@ -4470,6 +4500,9 @@
         <f t="shared" si="0"/>
         <v>7.2000000000000171</v>
       </c>
+      <c r="C41" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
@@ -4479,6 +4512,9 @@
         <f t="shared" si="0"/>
         <v>4.8000000000000167</v>
       </c>
+      <c r="C42" s="1">
+        <v>20</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -4487,6 +4523,9 @@
       <c r="B43" s="3">
         <f t="shared" si="0"/>
         <v>2.4000000000000168</v>
+      </c>
+      <c r="C43" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Sprint 1 Retrospective
</commit_message>
<xml_diff>
--- a/Group 68 Burndown Charts.xlsx
+++ b/Group 68 Burndown Charts.xlsx
@@ -613,6 +613,9 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
@@ -1172,6 +1175,9 @@
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4215,8 +4221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4262,6 +4268,9 @@
       <c r="B4" s="3">
         <v>30</v>
       </c>
+      <c r="C4" s="1">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -4534,6 +4543,9 @@
       </c>
       <c r="B44" s="1">
         <v>0</v>
+      </c>
+      <c r="C44" s="1">
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated User Stories, Updated Burndown Charts
</commit_message>
<xml_diff>
--- a/Group 68 Burndown Charts.xlsx
+++ b/Group 68 Burndown Charts.xlsx
@@ -274,20 +274,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'Burn down chart'!$A$24:$A$44</c:f>
@@ -1706,64 +1692,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>61</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.95</c:v>
+                  <c:v>45.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.900000000000006</c:v>
+                  <c:v>43.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.850000000000009</c:v>
+                  <c:v>40.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.800000000000011</c:v>
+                  <c:v>38.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45.750000000000014</c:v>
+                  <c:v>36.000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.700000000000017</c:v>
+                  <c:v>33.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.65000000000002</c:v>
+                  <c:v>31.20000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.600000000000023</c:v>
+                  <c:v>28.800000000000011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33.550000000000026</c:v>
+                  <c:v>26.400000000000013</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30.500000000000025</c:v>
+                  <c:v>24.000000000000014</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.450000000000024</c:v>
+                  <c:v>21.600000000000016</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.400000000000023</c:v>
+                  <c:v>19.200000000000017</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>21.350000000000023</c:v>
+                  <c:v>16.800000000000018</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.300000000000022</c:v>
+                  <c:v>14.400000000000018</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.250000000000021</c:v>
+                  <c:v>12.000000000000018</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>12.200000000000021</c:v>
+                  <c:v>9.6000000000000174</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9.1500000000000199</c:v>
+                  <c:v>7.2000000000000171</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.1000000000000201</c:v>
+                  <c:v>4.8000000000000167</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.0500000000000203</c:v>
+                  <c:v>2.4000000000000168</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1907,34 +1893,49 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>39</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>39</c:v>
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4320,8 +4321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4672,7 +4673,7 @@
         <v>20</v>
       </c>
       <c r="B48" s="1">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="C48" s="1">
         <v>61</v>
@@ -4684,8 +4685,8 @@
         <v>19</v>
       </c>
       <c r="B49" s="3">
-        <f>B48-3.05</f>
-        <v>57.95</v>
+        <f>B48-2.4</f>
+        <v>45.6</v>
       </c>
       <c r="C49" s="1">
         <v>61</v>
@@ -4697,8 +4698,8 @@
         <v>18</v>
       </c>
       <c r="B50" s="3">
-        <f t="shared" ref="B50:B67" si="1">B49-3.05</f>
-        <v>54.900000000000006</v>
+        <f t="shared" ref="B50:B68" si="1">B49-2.4</f>
+        <v>43.2</v>
       </c>
       <c r="C50" s="1">
         <v>61</v>
@@ -4711,7 +4712,7 @@
       </c>
       <c r="B51" s="3">
         <f t="shared" si="1"/>
-        <v>51.850000000000009</v>
+        <v>40.800000000000004</v>
       </c>
       <c r="C51" s="1">
         <v>61</v>
@@ -4724,11 +4725,10 @@
       </c>
       <c r="B52" s="3">
         <f t="shared" si="1"/>
-        <v>48.800000000000011</v>
+        <v>38.400000000000006</v>
       </c>
       <c r="C52" s="1">
-        <f>C51-6</f>
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D52" s="2"/>
     </row>
@@ -4738,10 +4738,10 @@
       </c>
       <c r="B53" s="3">
         <f t="shared" si="1"/>
-        <v>45.750000000000014</v>
+        <v>36.000000000000007</v>
       </c>
       <c r="C53" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D53" s="2"/>
     </row>
@@ -4751,10 +4751,10 @@
       </c>
       <c r="B54" s="3">
         <f t="shared" si="1"/>
-        <v>42.700000000000017</v>
+        <v>33.600000000000009</v>
       </c>
       <c r="C54" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D54" s="2"/>
     </row>
@@ -4764,10 +4764,10 @@
       </c>
       <c r="B55" s="3">
         <f t="shared" si="1"/>
-        <v>39.65000000000002</v>
+        <v>31.20000000000001</v>
       </c>
       <c r="C55" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D55" s="2"/>
     </row>
@@ -4777,10 +4777,10 @@
       </c>
       <c r="B56" s="3">
         <f t="shared" si="1"/>
-        <v>36.600000000000023</v>
+        <v>28.800000000000011</v>
       </c>
       <c r="C56" s="1">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D56" s="2"/>
     </row>
@@ -4790,11 +4790,11 @@
       </c>
       <c r="B57" s="3">
         <f t="shared" si="1"/>
-        <v>33.550000000000026</v>
+        <v>26.400000000000013</v>
       </c>
       <c r="C57" s="1">
         <f>C56-13</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D57" s="2"/>
     </row>
@@ -4804,10 +4804,10 @@
       </c>
       <c r="B58" s="3">
         <f t="shared" si="1"/>
-        <v>30.500000000000025</v>
+        <v>24.000000000000014</v>
       </c>
       <c r="C58" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -4816,10 +4816,10 @@
       </c>
       <c r="B59" s="3">
         <f t="shared" si="1"/>
-        <v>27.450000000000024</v>
+        <v>21.600000000000016</v>
       </c>
       <c r="C59" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -4828,10 +4828,10 @@
       </c>
       <c r="B60" s="3">
         <f t="shared" si="1"/>
-        <v>24.400000000000023</v>
+        <v>19.200000000000017</v>
       </c>
       <c r="C60" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -4840,10 +4840,10 @@
       </c>
       <c r="B61" s="3">
         <f t="shared" si="1"/>
-        <v>21.350000000000023</v>
+        <v>16.800000000000018</v>
       </c>
       <c r="C61" s="1">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -4852,7 +4852,10 @@
       </c>
       <c r="B62" s="3">
         <f t="shared" si="1"/>
-        <v>18.300000000000022</v>
+        <v>14.400000000000018</v>
+      </c>
+      <c r="C62" s="1">
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -4861,7 +4864,10 @@
       </c>
       <c r="B63" s="3">
         <f t="shared" si="1"/>
-        <v>15.250000000000021</v>
+        <v>12.000000000000018</v>
+      </c>
+      <c r="C63" s="1">
+        <v>34</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -4870,7 +4876,10 @@
       </c>
       <c r="B64" s="3">
         <f t="shared" si="1"/>
-        <v>12.200000000000021</v>
+        <v>9.6000000000000174</v>
+      </c>
+      <c r="C64" s="1">
+        <v>34</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -4879,7 +4888,10 @@
       </c>
       <c r="B65" s="3">
         <f t="shared" si="1"/>
-        <v>9.1500000000000199</v>
+        <v>7.2000000000000171</v>
+      </c>
+      <c r="C65" s="1">
+        <v>30</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -4888,7 +4900,10 @@
       </c>
       <c r="B66" s="3">
         <f t="shared" si="1"/>
-        <v>6.1000000000000201</v>
+        <v>4.8000000000000167</v>
+      </c>
+      <c r="C66" s="1">
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -4897,7 +4912,7 @@
       </c>
       <c r="B67" s="3">
         <f t="shared" si="1"/>
-        <v>3.0500000000000203</v>
+        <v>2.4000000000000168</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Final Release & Sprint Plan, Added Test Cases, Updated Burndown Charts
</commit_message>
<xml_diff>
--- a/Group 68 Burndown Charts.xlsx
+++ b/Group 68 Burndown Charts.xlsx
@@ -1165,6 +1165,9 @@
                 <c:pt idx="1">
                   <c:v>60</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1941,7 +1944,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4327,8 +4330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -4385,6 +4388,9 @@
       <c r="B5" s="3">
         <v>0</v>
       </c>
+      <c r="C5" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
@@ -4932,7 +4938,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="1">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">

</xml_diff>